<commit_message>
Add clickable names to allow to checking of person location
</commit_message>
<xml_diff>
--- a/photos/AlbumInfo.xlsx
+++ b/photos/AlbumInfo.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,10 +481,15 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
+          <t>people_rgb</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
           <t>complete</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>lastedit</t>
         </is>
@@ -532,17 +537,22 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>(173,106)|(493,588)|(784,135)|</t>
+          <t>(176,94)|(478,589)|(783,136)|</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
+          <t>(0, 0, 0, 1)|(0, 0, 0, 1)|(0, 0, 0, 1)|</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
           <t>Y</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>03/01/2023 20:22:05</t>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>05/01/2023 16:30:13</t>
         </is>
       </c>
     </row>

</xml_diff>